<commit_message>
Update Leetcode Progress and Notes.xlsx
</commit_message>
<xml_diff>
--- a/Leetcode Progress and Notes.xlsx
+++ b/Leetcode Progress and Notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kenzo\Desktop\Git\Leetcode-HackerRank\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7450C2FB-56F9-47DF-BEA0-7728E525E7F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0663DE0-AACC-420C-A2AD-6EC0B1CD10EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14850" xr2:uid="{21E4B2D5-1FE5-41BA-B509-B73F7C4738BF}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Category</t>
   </si>
@@ -73,6 +73,15 @@
       </rPr>
       <t>To do LRU cache to add add/delete methonds</t>
     </r>
+  </si>
+  <si>
+    <t>Similar problems</t>
+  </si>
+  <si>
+    <t>215. Kth Largest Element in an Array</t>
+  </si>
+  <si>
+    <t>Minimum Size Subarray Sum</t>
   </si>
 </sst>
 </file>
@@ -102,10 +111,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color rgb="FF212121"/>
-      <name val="Segoe UI"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -131,8 +141,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C7BA473-9CB4-49B6-8414-78179D0A27A3}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,11 +468,11 @@
     <col min="2" max="2" width="38.28515625" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
     <col min="4" max="4" width="39" customWidth="1"/>
-    <col min="5" max="5" width="50.42578125" customWidth="1"/>
+    <col min="5" max="5" width="51.85546875" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -471,7 +481,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -487,15 +497,18 @@
       <c r="E2" t="s">
         <v>5</v>
       </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>230</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>43761</v>
       </c>
       <c r="D3" t="s">
@@ -503,6 +516,17 @@
       </c>
       <c r="E3" t="s">
         <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>209</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>